<commit_message>
Adicionando Extent Reports ao projeto
</commit_message>
<xml_diff>
--- a/CadastroComDadosExcel.xlsx
+++ b/CadastroComDadosExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rsiinf-my.sharepoint.com/personal/fernando_fernandes_keeggo_com/Documents/Documentos/Pastas Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fernando.fernandes\2019-selenium-java-projeto_inicial\AdvantageDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{1C7FEF1D-6535-4606-B9AD-36C21B43C381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2165F3B-ED08-4C7B-90AB-5879F8A15291}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9448F4-4221-47C4-8B21-2DF24339B3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8C84741D-0272-4A74-886D-7012E70268FE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{8C84741D-0272-4A74-886D-7012E70268FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -100,13 +100,13 @@
     <t>fernando22@testando.com</t>
   </si>
   <si>
-    <t>Fernando301</t>
-  </si>
-  <si>
     <t>11989272724</t>
   </si>
   <si>
     <t>6364001</t>
+  </si>
+  <si>
+    <t>Fernando304</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,7 +540,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>20</v>
@@ -558,7 +558,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>15</v>
@@ -573,7 +573,7 @@
         <v>16</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M2" s="1"/>
     </row>
@@ -597,7 +597,7 @@
         <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>15</v>
@@ -612,7 +612,7 @@
         <v>16</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M3" s="1"/>
     </row>

</xml_diff>